<commit_message>
cleaned up team writeouts
</commit_message>
<xml_diff>
--- a/replacement/replacement_pitchers.xlsx
+++ b/replacement/replacement_pitchers.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\replacement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:140008_{9800BFB8-5F52-4EE6-869C-69B7C1EA3217}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8A6F889-DF80-4C42-9744-D232F61505AF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="replacement" sheetId="2" r:id="rId1"/>
     <sheet name="source" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -989,11 +989,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>